<commit_message>
updated ..\tests\data and ..\tests\images
</commit_message>
<xml_diff>
--- a/tests/data/dat.xlsx
+++ b/tests/data/dat.xlsx
@@ -66,6 +66,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 

</xml_diff>

<commit_message>
update data for tests
</commit_message>
<xml_diff>
--- a/tests/data/dat.xlsx
+++ b/tests/data/dat.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TestSheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TestSheet11" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TestSheet21" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="TestSheet12" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TestSheet22" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet11" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet21" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet12" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet22" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Overwrite all due to backup crashes
</commit_message>
<xml_diff>
--- a/tests/data/dat.xlsx
+++ b/tests/data/dat.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet11" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet21" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet12" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestSheet22" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="TestSheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TestSheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TestSheet11" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TestSheet21" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="TestSheet12" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TestSheet22" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>